<commit_message>
Actualiza planilla de binomio
</commit_message>
<xml_diff>
--- a/Test Rendimiento Binomio Newton.xlsx
+++ b/Test Rendimiento Binomio Newton.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>terminoK Iterativo</t>
   </si>
@@ -36,6 +36,12 @@
   </si>
   <si>
     <t>desarrolloCompleto Recursivo</t>
+  </si>
+  <si>
+    <t>terminoK Mejorado</t>
+  </si>
+  <si>
+    <t>desarrolloCompleto Mejorado</t>
   </si>
 </sst>
 </file>
@@ -164,11 +170,11 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="es-AR"/>
-              <a:t>Test</a:t>
+              <a:t>Test rendimiento</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="es-AR" baseline="0"/>
-              <a:t> término K</a:t>
+              <a:t> termino K</a:t>
             </a:r>
             <a:endParaRPr lang="es-AR"/>
           </a:p>
@@ -208,7 +214,7 @@
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
-        <c:grouping val="stacked"/>
+        <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -446,406 +452,16 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="187133520"/>
-        <c:axId val="187132960"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="187133520"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="es-AR"/>
-                  <a:t>Grado</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="es-AR" baseline="0"/>
-                  <a:t> binomio</a:t>
-                </a:r>
-                <a:endParaRPr lang="es-AR"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="es-AR"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="es-AR"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="187132960"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="187132960"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="es-AR"/>
-                  <a:t>Milisegundos</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="es-AR"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="low"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="es-AR"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="187133520"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="es-AR"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="zero"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="es-AR"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="es-AR"/>
-              <a:t>Test desarrollo completo</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="es-AR"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="stacked"/>
-        <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
+          <c:idx val="2"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
               <c:f>Hoja1!$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>desarrolloCompleto Iterativo</c:v>
+                  <c:v>terminoK Mejorado</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -853,7 +469,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent3"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -864,11 +480,11 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent3"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:schemeClr val="accent3"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -948,124 +564,6 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Hoja1!$A$5</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>desarrolloCompleto Recursivo</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Hoja1!$B$1:$K$1</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>34</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>36</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Hoja1!$B$5:$K$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>67</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1024385</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1738630</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>4466686</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1082,11 +580,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="280690704"/>
-        <c:axId val="185355520"/>
+        <c:axId val="239065792"/>
+        <c:axId val="239064112"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="280690704"/>
+        <c:axId val="239065792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1185,7 +683,7 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="185355520"/>
+        <c:crossAx val="239064112"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1193,7 +691,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="185355520"/>
+        <c:axId val="239064112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1300,7 +798,7 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="280690704"/>
+        <c:crossAx val="239065792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1345,7 +843,633 @@
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="zero"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-AR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-AR"/>
+              <a:t>Test</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="es-AR" baseline="0"/>
+              <a:t> rendimiento desarrollo completo</a:t>
+            </a:r>
+            <a:endParaRPr lang="es-AR"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-AR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>desarrolloCompleto Iterativo</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$B$5:$K$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>desarrolloCompleto Recursivo</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$B$6:$K$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1024385</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1738630</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4466686</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>desarrolloCompleto Mejorado</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$B$7:$K$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="241349472"/>
+        <c:axId val="242138272"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="241349472"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-AR"/>
+                  <a:t>Grado binomio</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-AR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-AR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="242138272"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="242138272"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-AR"/>
+                  <a:t>Milisegundos</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-AR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-AR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="241349472"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-AR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
@@ -2472,19 +2596,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>185737</xdr:rowOff>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>71437</xdr:rowOff>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvPr id="5" name="Gráfico 4"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2502,19 +2626,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>4762</xdr:rowOff>
+      <xdr:colOff>14287</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>80962</xdr:rowOff>
+      <xdr:colOff>14287</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Gráfico 2"/>
+        <xdr:cNvPr id="6" name="Gráfico 5"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2795,10 +2919,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2911,7 +3035,7 @@
     </row>
     <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B4" s="3">
         <v>0</v>
@@ -2946,37 +3070,107 @@
     </row>
     <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0</v>
+      </c>
+      <c r="H5" s="3">
+        <v>0</v>
+      </c>
+      <c r="I5" s="3">
+        <v>0</v>
+      </c>
+      <c r="J5" s="3">
+        <v>0</v>
+      </c>
+      <c r="K5" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="3">
-        <v>0</v>
-      </c>
-      <c r="C5" s="3">
-        <v>0</v>
-      </c>
-      <c r="D5" s="3">
-        <v>0</v>
-      </c>
-      <c r="E5" s="3">
-        <v>0</v>
-      </c>
-      <c r="F5" s="3">
-        <v>0</v>
-      </c>
-      <c r="G5" s="3">
+      <c r="B6" s="3">
+        <v>0</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0</v>
+      </c>
+      <c r="G6" s="3">
         <v>1</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H6" s="3">
         <v>67</v>
       </c>
-      <c r="I5" s="3">
+      <c r="I6" s="3">
         <v>1024385</v>
       </c>
-      <c r="J5" s="3">
+      <c r="J6" s="3">
         <v>1738630</v>
       </c>
-      <c r="K5" s="3">
+      <c r="K6" s="3">
         <v>4466686</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0</v>
+      </c>
+      <c r="H7" s="3">
+        <v>0</v>
+      </c>
+      <c r="I7" s="3">
+        <v>0</v>
+      </c>
+      <c r="J7" s="3">
+        <v>0</v>
+      </c>
+      <c r="K7" s="3">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>